<commit_message>
Modifique el pan de fiesta
</commit_message>
<xml_diff>
--- a/Fiesta/Plan_Fiesta.xlsx
+++ b/Fiesta/Plan_Fiesta.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Asignado</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>ya lo hice</t>
+  </si>
+  <si>
+    <t>Tlapa</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -174,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,10 +424,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="2" customWidth="1"/>
@@ -468,10 +471,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Nueva modificacion de nombre
</commit_message>
<xml_diff>
--- a/Fiesta/Plan_Fiesta.xlsx
+++ b/Fiesta/Plan_Fiesta.xlsx
@@ -55,7 +55,7 @@
     <t>ya lo hice</t>
   </si>
   <si>
-    <t>Tlapa</t>
+    <t>Rodrigo Tlapa</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>

</xml_diff>